<commit_message>
Addition of Mapping API
</commit_message>
<xml_diff>
--- a/Testing/Testcase_1.xlsx
+++ b/Testing/Testcase_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\80951259\Documents\SaiVineelaPeddinti\github\AI_DataModeler1\AI_DATAMODELER\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/80951259/Documents/Lakshmikanth/Personal/Vineela/AI_DATAMODELER-main/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7CBA72-93EC-4C7B-A5B6-A732B5B5DC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFC9E4B-5B6E-154B-B1DD-4D39D3A7400E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="5280" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DRD" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="431">
   <si>
     <t>order_id</t>
   </si>
@@ -1290,19 +1290,55 @@
   </si>
   <si>
     <t>Orders data from Sales Team</t>
+  </si>
+  <si>
+    <t>customer_orders</t>
+  </si>
+  <si>
+    <t>Order Management</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>Customer Info</t>
+  </si>
+  <si>
+    <t>source_table</t>
+  </si>
+  <si>
+    <t>source_column</t>
+  </si>
+  <si>
+    <t>source_data_type</t>
+  </si>
+  <si>
+    <t>source_column_description</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA2FCA2"/>
+      <name val="Consolas"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1325,9 +1361,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1614,14 +1651,14 @@
       <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>416</v>
       </c>
@@ -1632,7 +1669,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>419</v>
       </c>
@@ -1643,7 +1680,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>419</v>
       </c>
@@ -1654,7 +1691,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>419</v>
       </c>
@@ -1665,7 +1702,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>419</v>
       </c>
@@ -1676,7 +1713,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>419</v>
       </c>
@@ -1687,7 +1724,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>419</v>
       </c>
@@ -1698,7 +1735,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>419</v>
       </c>
@@ -1709,7 +1746,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>419</v>
       </c>
@@ -1720,7 +1757,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>419</v>
       </c>
@@ -1731,7 +1768,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>419</v>
       </c>
@@ -1742,7 +1779,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>419</v>
       </c>
@@ -1753,7 +1790,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>419</v>
       </c>
@@ -1764,7 +1801,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>419</v>
       </c>
@@ -1775,7 +1812,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>419</v>
       </c>
@@ -1786,7 +1823,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>419</v>
       </c>
@@ -1797,7 +1834,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>419</v>
       </c>
@@ -1808,7 +1845,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>419</v>
       </c>
@@ -1819,7 +1856,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>419</v>
       </c>
@@ -1830,7 +1867,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>419</v>
       </c>
@@ -1841,7 +1878,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>419</v>
       </c>
@@ -1861,16 +1898,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BF6D68-E507-4075-9ED8-DD7114F9F4B9}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1969,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1994,7 +2031,7 @@
         <v>898.72</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2056,7 +2093,7 @@
         <v>446.37</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2118,7 +2155,7 @@
         <v>101.55</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -2180,7 +2217,7 @@
         <v>264.14999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -2242,7 +2279,7 @@
         <v>937.54</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -2304,7 +2341,7 @@
         <v>156.80000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -2366,7 +2403,7 @@
         <v>811.78</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -2428,7 +2465,7 @@
         <v>181.03</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -2490,7 +2527,7 @@
         <v>413.64</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -2552,7 +2589,7 @@
         <v>369.44</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>103</v>
       </c>
@@ -2614,7 +2651,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>111</v>
       </c>
@@ -2676,7 +2713,7 @@
         <v>216.73</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -2738,7 +2775,7 @@
         <v>911.63</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -2800,7 +2837,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>134</v>
       </c>
@@ -2862,7 +2899,7 @@
         <v>138.77000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>142</v>
       </c>
@@ -2924,7 +2961,7 @@
         <v>51.76</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>150</v>
       </c>
@@ -2986,7 +3023,7 @@
         <v>333.12</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -3048,7 +3085,7 @@
         <v>264.27999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>166</v>
       </c>
@@ -3110,7 +3147,7 @@
         <v>806.22</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -3172,7 +3209,7 @@
         <v>31.29</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -3234,7 +3271,7 @@
         <v>834.47</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>190</v>
       </c>
@@ -3296,7 +3333,7 @@
         <v>380.49</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>197</v>
       </c>
@@ -3358,7 +3395,7 @@
         <v>271.20999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>205</v>
       </c>
@@ -3420,7 +3457,7 @@
         <v>152.5</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>211</v>
       </c>
@@ -3482,7 +3519,7 @@
         <v>182.86</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>219</v>
       </c>
@@ -3544,7 +3581,7 @@
         <v>914.63</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>227</v>
       </c>
@@ -3606,7 +3643,7 @@
         <v>67.069999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>235</v>
       </c>
@@ -3668,7 +3705,7 @@
         <v>387.23</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>243</v>
       </c>
@@ -3730,7 +3767,7 @@
         <v>98.26</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>251</v>
       </c>
@@ -3792,7 +3829,7 @@
         <v>213.13</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>259</v>
       </c>
@@ -3854,7 +3891,7 @@
         <v>811.29</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>267</v>
       </c>
@@ -3916,7 +3953,7 @@
         <v>65.48</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>275</v>
       </c>
@@ -3978,7 +4015,7 @@
         <v>705.04</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>283</v>
       </c>
@@ -4040,7 +4077,7 @@
         <v>175.22</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>291</v>
       </c>
@@ -4102,7 +4139,7 @@
         <v>217.43</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>299</v>
       </c>
@@ -4164,7 +4201,7 @@
         <v>651.05999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>306</v>
       </c>
@@ -4226,7 +4263,7 @@
         <v>391.08</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>314</v>
       </c>
@@ -4288,7 +4325,7 @@
         <v>823.75</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>322</v>
       </c>
@@ -4350,7 +4387,7 @@
         <v>953.36</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>330</v>
       </c>
@@ -4412,7 +4449,7 @@
         <v>304.57</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>338</v>
       </c>
@@ -4474,7 +4511,7 @@
         <v>184.89</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>345</v>
       </c>
@@ -4536,7 +4573,7 @@
         <v>371.74</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>353</v>
       </c>
@@ -4598,7 +4635,7 @@
         <v>424.26</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>360</v>
       </c>
@@ -4660,7 +4697,7 @@
         <v>46.98</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>368</v>
       </c>
@@ -4722,7 +4759,7 @@
         <v>481.12</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>376</v>
       </c>
@@ -4784,7 +4821,7 @@
         <v>227.9</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>384</v>
       </c>
@@ -4846,7 +4883,7 @@
         <v>357.36</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>392</v>
       </c>
@@ -4908,7 +4945,7 @@
         <v>932.22</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>400</v>
       </c>
@@ -4970,7 +5007,7 @@
         <v>676.16</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>408</v>
       </c>
@@ -5039,12 +5076,62 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58421D6-1596-46B2-9B9C-638A6D6128F7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>